<commit_message>
wrote the script fro all contracts but values not matching
</commit_message>
<xml_diff>
--- a/mstable.xlsx
+++ b/mstable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\clickdee\mStable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5DDAF3A-3AEB-46AB-A124-49DA24A0C974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F056C0-15C4-4D37-805E-14A2F3D3F21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E04F9DBC-75EA-4345-88DE-C1D61A0C748E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t xml:space="preserve">Protocol </t>
   </si>
@@ -137,6 +137,9 @@
       </rPr>
       <t xml:space="preserve"> section)</t>
     </r>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,21 +547,33 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>9</v>
       </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -569,45 +584,63 @@
       <c r="B13" t="s">
         <v>15</v>
       </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>19</v>
       </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>